<commit_message>
Replaced all the text for the new files created
</commit_message>
<xml_diff>
--- a/source/2015 Master Product Listing Clay Internet.xlsx
+++ b/source/2015 Master Product Listing Clay Internet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51195" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Full Head Masks" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="Albino_Ghoul" localSheetId="4">Makeup!#REF!</definedName>
     <definedName name="Albino_Ghoul">'Full Head Masks'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -682,7 +682,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -720,6 +720,12 @@
       <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor rgb="FF99CCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -927,7 +933,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -942,10 +948,6 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="44" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -977,7 +979,6 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1073,6 +1074,47 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="111">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1455,7 +1497,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1469,22 +1511,22 @@
   <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="82.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" style="19" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="19" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="4" hidden="1" customWidth="1"/>
-    <col min="7" max="16384" width="17.33203125" style="3"/>
+    <col min="1" max="1" width="82.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="18" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="18" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="7" max="16384" width="17.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" customHeight="1" thickBot="1">
+    <row r="1" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1497,1116 +1539,1116 @@
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="50" t="s">
         <v>179</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="51" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:6" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="56">
         <v>20</v>
       </c>
-      <c r="D2" s="40">
+      <c r="D2" s="57">
         <v>39.99</v>
       </c>
-      <c r="E2" s="39"/>
-      <c r="F2" s="49"/>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
-      <c r="A3" s="6" t="s">
+      <c r="E2" s="58"/>
+      <c r="F2" s="59"/>
+    </row>
+    <row r="3" spans="1:6" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="56">
         <v>30</v>
       </c>
-      <c r="D3" s="40">
+      <c r="D3" s="57">
         <v>59.99</v>
       </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="49"/>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
-      <c r="A4" s="6" t="s">
+      <c r="E3" s="58"/>
+      <c r="F3" s="59"/>
+    </row>
+    <row r="4" spans="1:6" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="55" t="s">
         <v>181</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="56">
         <v>24</v>
       </c>
-      <c r="D4" s="40">
+      <c r="D4" s="57">
         <v>49.99</v>
       </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="49"/>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1">
-      <c r="A5" s="6" t="s">
+      <c r="E4" s="58"/>
+      <c r="F4" s="59"/>
+    </row>
+    <row r="5" spans="1:6" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="56">
         <v>39.5</v>
       </c>
-      <c r="D5" s="40">
+      <c r="D5" s="57">
         <v>79.989999999999995</v>
       </c>
-      <c r="E5" s="39"/>
-      <c r="F5" s="49"/>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1">
-      <c r="A6" s="6" t="s">
+      <c r="E5" s="58"/>
+      <c r="F5" s="59"/>
+    </row>
+    <row r="6" spans="1:6" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="54" t="s">
         <v>158</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="55" t="s">
         <v>159</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="56">
         <v>12</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="57">
         <v>24.99</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="49"/>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1">
-      <c r="A7" s="6" t="s">
+      <c r="E6" s="58"/>
+      <c r="F6" s="59"/>
+    </row>
+    <row r="7" spans="1:6" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="54" t="s">
         <v>193</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="55" t="s">
         <v>182</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="56">
         <v>39.5</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="57">
         <v>79.989999999999995</v>
       </c>
-      <c r="E7" s="39"/>
-      <c r="F7" s="49"/>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1">
-      <c r="A8" s="6" t="s">
+      <c r="E7" s="58"/>
+      <c r="F7" s="59"/>
+    </row>
+    <row r="8" spans="1:6" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="56">
         <v>26.5</v>
       </c>
-      <c r="D8" s="40">
+      <c r="D8" s="57">
         <v>54.99</v>
       </c>
-      <c r="E8" s="39"/>
-      <c r="F8" s="49"/>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1">
-      <c r="A9" s="11" t="s">
+      <c r="E8" s="58"/>
+      <c r="F8" s="59"/>
+    </row>
+    <row r="9" spans="1:6" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="61" t="s">
         <v>145</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="56">
         <v>56</v>
       </c>
-      <c r="D9" s="40">
+      <c r="D9" s="57">
         <f>C9*2</f>
         <v>112</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="49"/>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1">
-      <c r="A10" s="6" t="s">
+      <c r="E9" s="58"/>
+      <c r="F9" s="59"/>
+    </row>
+    <row r="10" spans="1:6" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="55" t="s">
         <v>153</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="56">
         <v>34.5</v>
       </c>
-      <c r="D10" s="40">
+      <c r="D10" s="57">
         <v>69.989999999999995</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="49"/>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1">
-      <c r="A11" s="6" t="s">
+      <c r="E10" s="58"/>
+      <c r="F10" s="59"/>
+    </row>
+    <row r="11" spans="1:6" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="56">
         <v>42</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="57">
         <f>C11*2</f>
         <v>84</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="49"/>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1">
-      <c r="A12" s="13" t="s">
+      <c r="E11" s="58"/>
+      <c r="F11" s="59"/>
+    </row>
+    <row r="12" spans="1:6" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="63" t="s">
         <v>132</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="63" t="s">
         <v>133</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="64">
         <v>20</v>
       </c>
-      <c r="D12" s="38">
+      <c r="D12" s="65">
         <v>39.99</v>
       </c>
-      <c r="E12" s="39"/>
-      <c r="F12" s="49"/>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1">
-      <c r="A13" s="6" t="s">
+      <c r="E12" s="58"/>
+      <c r="F12" s="59"/>
+    </row>
+    <row r="13" spans="1:6" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="55" t="s">
         <v>164</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="56">
         <v>28.5</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="64">
         <v>59.99</v>
       </c>
-      <c r="E13" s="39"/>
-      <c r="F13" s="49"/>
-    </row>
-    <row r="14" spans="1:6" ht="19" customHeight="1">
-      <c r="A14" s="6" t="s">
+      <c r="E13" s="58"/>
+      <c r="F13" s="59"/>
+    </row>
+    <row r="14" spans="1:6" s="60" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="54" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="56">
         <v>64</v>
       </c>
-      <c r="D14" s="40">
+      <c r="D14" s="57">
         <f>C14*2</f>
         <v>128</v>
       </c>
-      <c r="E14" s="39"/>
-      <c r="F14" s="49"/>
-    </row>
-    <row r="15" spans="1:6" ht="24" customHeight="1">
-      <c r="A15" s="6" t="s">
+      <c r="E14" s="58"/>
+      <c r="F14" s="59"/>
+    </row>
+    <row r="15" spans="1:6" s="60" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="54" t="s">
         <v>178</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="55" t="s">
         <v>177</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="56">
         <v>32</v>
       </c>
-      <c r="D15" s="40">
+      <c r="D15" s="57">
         <v>59.99</v>
       </c>
-      <c r="E15" s="39"/>
-      <c r="F15" s="49"/>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1">
-      <c r="A16" s="6" t="s">
+      <c r="E15" s="58"/>
+      <c r="F15" s="59"/>
+    </row>
+    <row r="16" spans="1:6" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="56">
         <v>23</v>
       </c>
-      <c r="D16" s="40">
+      <c r="D16" s="57">
         <v>49.99</v>
       </c>
-      <c r="E16" s="39"/>
-      <c r="F16" s="49"/>
-    </row>
-    <row r="17" spans="1:7" ht="20" customHeight="1">
-      <c r="A17" s="17" t="s">
+      <c r="E16" s="58"/>
+      <c r="F16" s="59"/>
+    </row>
+    <row r="17" spans="1:7" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="66" t="s">
         <v>183</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="67">
         <v>22</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="64">
         <v>49.99</v>
       </c>
-      <c r="E17" s="39"/>
-      <c r="F17" s="49"/>
-    </row>
-    <row r="18" spans="1:7" ht="20" customHeight="1">
-      <c r="A18" s="17" t="s">
+      <c r="E17" s="58"/>
+      <c r="F17" s="59"/>
+    </row>
+    <row r="18" spans="1:7" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="67">
         <v>25</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="64">
         <v>49.99</v>
       </c>
-      <c r="E18" s="39"/>
-      <c r="F18" s="49"/>
-    </row>
-    <row r="19" spans="1:7" ht="20" customHeight="1">
-      <c r="A19" s="17" t="s">
+      <c r="E18" s="58"/>
+      <c r="F18" s="59"/>
+    </row>
+    <row r="19" spans="1:7" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="67">
         <v>22</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="64">
         <v>49.99</v>
       </c>
-      <c r="E19" s="39"/>
-      <c r="F19" s="49"/>
-    </row>
-    <row r="20" spans="1:7" ht="20" customHeight="1">
-      <c r="A20" s="6" t="s">
+      <c r="E19" s="58"/>
+      <c r="F19" s="59"/>
+    </row>
+    <row r="20" spans="1:7" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="56">
         <v>28.5</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="64">
         <v>59.99</v>
       </c>
-      <c r="E20" s="39"/>
-      <c r="F20" s="49"/>
-    </row>
-    <row r="21" spans="1:7" ht="20" customHeight="1">
-      <c r="A21" s="20" t="s">
+      <c r="E20" s="58"/>
+      <c r="F20" s="59"/>
+    </row>
+    <row r="21" spans="1:7" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="63" t="s">
         <v>144</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="64">
         <v>23</v>
       </c>
-      <c r="D21" s="38">
+      <c r="D21" s="65">
         <f>C21*2</f>
         <v>46</v>
       </c>
-      <c r="E21" s="39"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:7" ht="20" customHeight="1">
-      <c r="A22" s="20" t="s">
+      <c r="E21" s="58"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="68"/>
+    </row>
+    <row r="22" spans="1:7" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="63" t="s">
         <v>139</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="63" t="s">
         <v>140</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="64">
         <v>26</v>
       </c>
-      <c r="D22" s="38">
+      <c r="D22" s="65">
         <f>C22*2</f>
         <v>52</v>
       </c>
-      <c r="E22" s="39"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="1:7" ht="20" customHeight="1">
-      <c r="A23" s="20" t="s">
+      <c r="E22" s="58"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="68"/>
+    </row>
+    <row r="23" spans="1:7" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="63" t="s">
         <v>142</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="63" t="s">
         <v>141</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="64">
         <v>23</v>
       </c>
-      <c r="D23" s="38">
+      <c r="D23" s="65">
         <f>C23*2</f>
         <v>46</v>
       </c>
-      <c r="E23" s="39"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="1:7" ht="20" customHeight="1">
-      <c r="A24" s="20" t="s">
+      <c r="E23" s="58"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="68"/>
+    </row>
+    <row r="24" spans="1:7" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="63" t="s">
         <v>138</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="63" t="s">
         <v>137</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="64">
         <v>28</v>
       </c>
-      <c r="D24" s="38">
+      <c r="D24" s="65">
         <f>C24*2</f>
         <v>56</v>
       </c>
-      <c r="E24" s="39"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="1:7" ht="20" customHeight="1">
-      <c r="A25" s="21" t="s">
+      <c r="E24" s="58"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="68"/>
+    </row>
+    <row r="25" spans="1:7" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="14">
+      <c r="C25" s="64">
         <v>29.5</v>
       </c>
-      <c r="D25" s="38">
+      <c r="D25" s="65">
         <v>59.99</v>
       </c>
-      <c r="E25" s="39"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="4"/>
-    </row>
-    <row r="26" spans="1:7" ht="20" customHeight="1">
-      <c r="A26" s="21" t="s">
+      <c r="E25" s="58"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="68"/>
+    </row>
+    <row r="26" spans="1:7" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="64">
         <v>29.5</v>
       </c>
-      <c r="D26" s="38">
+      <c r="D26" s="65">
         <v>59.99</v>
       </c>
-      <c r="E26" s="39"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="1:7" ht="20" customHeight="1">
-      <c r="A27" s="21" t="s">
+      <c r="E26" s="58"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="68"/>
+    </row>
+    <row r="27" spans="1:7" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="69" t="s">
         <v>163</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="14">
+      <c r="C27" s="64">
         <v>22</v>
       </c>
-      <c r="D27" s="38">
+      <c r="D27" s="65">
         <f>C27*2</f>
         <v>44</v>
       </c>
-      <c r="E27" s="39"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="1:7" ht="20" customHeight="1">
-      <c r="A28" s="21" t="s">
+      <c r="E27" s="58"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="68"/>
+    </row>
+    <row r="28" spans="1:7" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="14">
+      <c r="C28" s="64">
         <v>26.5</v>
       </c>
-      <c r="D28" s="38">
+      <c r="D28" s="65">
         <v>54.99</v>
       </c>
-      <c r="E28" s="39"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="1:7" ht="20" customHeight="1">
-      <c r="A29" s="6" t="s">
+      <c r="E28" s="58"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="68"/>
+    </row>
+    <row r="29" spans="1:7" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="56">
         <v>28.5</v>
       </c>
-      <c r="D29" s="38">
+      <c r="D29" s="65">
         <v>59.99</v>
       </c>
-      <c r="E29" s="39"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="4"/>
-    </row>
-    <row r="30" spans="1:7" ht="20" customHeight="1">
-      <c r="A30" s="6" t="s">
+      <c r="E29" s="58"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="68"/>
+    </row>
+    <row r="30" spans="1:7" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="56">
         <v>30</v>
       </c>
-      <c r="D30" s="38">
+      <c r="D30" s="65">
         <v>59.99</v>
       </c>
-      <c r="E30" s="39"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="1:7" ht="20" customHeight="1">
-      <c r="A31" s="6" t="s">
+      <c r="E30" s="58"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="68"/>
+    </row>
+    <row r="31" spans="1:7" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="56">
         <v>30</v>
       </c>
-      <c r="D31" s="38">
+      <c r="D31" s="65">
         <v>59.99</v>
       </c>
-      <c r="E31" s="39"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="4"/>
-    </row>
-    <row r="32" spans="1:7" ht="20" customHeight="1">
-      <c r="A32" s="6" t="s">
+      <c r="E31" s="58"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="68"/>
+    </row>
+    <row r="32" spans="1:7" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="56">
         <v>27</v>
       </c>
-      <c r="D32" s="38">
+      <c r="D32" s="65">
         <f>C32*2</f>
         <v>54</v>
       </c>
-      <c r="E32" s="21"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="16"/>
-    </row>
-    <row r="33" spans="1:7" ht="20" customHeight="1">
-      <c r="A33" s="6" t="s">
+      <c r="E32" s="69"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="71"/>
+    </row>
+    <row r="33" spans="1:7" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="56">
         <v>25</v>
       </c>
-      <c r="D33" s="38">
+      <c r="D33" s="65">
         <v>49.99</v>
       </c>
-      <c r="E33" s="39"/>
-      <c r="F33" s="49"/>
-    </row>
-    <row r="34" spans="1:7" ht="20" customHeight="1">
-      <c r="A34" s="6" t="s">
+      <c r="E33" s="58"/>
+      <c r="F33" s="59"/>
+    </row>
+    <row r="34" spans="1:7" s="60" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="56">
         <v>39.5</v>
       </c>
-      <c r="D34" s="38">
+      <c r="D34" s="65">
         <v>79.989999999999995</v>
       </c>
-      <c r="E34" s="39"/>
-      <c r="F34" s="49"/>
-    </row>
-    <row r="35" spans="1:7" ht="20" customHeight="1">
+      <c r="E34" s="58"/>
+      <c r="F34" s="59"/>
+    </row>
+    <row r="35" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C35" s="7">
         <v>33</v>
       </c>
-      <c r="D35" s="38">
+      <c r="D35" s="36">
         <f>C35*2</f>
         <v>66</v>
       </c>
-      <c r="E35" s="39"/>
-      <c r="F35" s="49"/>
-    </row>
-    <row r="36" spans="1:7" ht="20" customHeight="1">
+      <c r="E35" s="37"/>
+      <c r="F35" s="47"/>
+    </row>
+    <row r="36" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="23" t="s">
+      <c r="B36" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C36" s="7">
         <v>33</v>
       </c>
-      <c r="D36" s="38">
+      <c r="D36" s="36">
         <f>C36*2</f>
         <v>66</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="49"/>
-    </row>
-    <row r="37" spans="1:7" ht="20" customHeight="1">
+      <c r="E36" s="37"/>
+      <c r="F36" s="47"/>
+    </row>
+    <row r="37" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B37" s="23" t="s">
+      <c r="B37" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37" s="7">
         <v>30</v>
       </c>
-      <c r="D37" s="38">
+      <c r="D37" s="36">
         <v>59.99</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="49"/>
-    </row>
-    <row r="38" spans="1:7" ht="20" customHeight="1">
+      <c r="E37" s="37"/>
+      <c r="F37" s="47"/>
+    </row>
+    <row r="38" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38" s="7">
         <v>32</v>
       </c>
-      <c r="D38" s="43">
+      <c r="D38" s="41">
         <v>59.99</v>
       </c>
-      <c r="E38" s="39"/>
-      <c r="F38" s="49"/>
-    </row>
-    <row r="39" spans="1:7" ht="20" customHeight="1">
-      <c r="A39" s="26" t="s">
+      <c r="E38" s="37"/>
+      <c r="F38" s="47"/>
+    </row>
+    <row r="39" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="28">
+      <c r="C39" s="26">
         <v>28.5</v>
       </c>
-      <c r="D39" s="45">
+      <c r="D39" s="43">
         <v>59.99</v>
       </c>
-      <c r="E39" s="39"/>
-      <c r="F39" s="49"/>
-    </row>
-    <row r="40" spans="1:7" ht="20" customHeight="1">
-      <c r="A40" s="26" t="s">
+      <c r="E39" s="37"/>
+      <c r="F39" s="47"/>
+    </row>
+    <row r="40" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C40" s="28">
+      <c r="C40" s="26">
         <v>30</v>
       </c>
-      <c r="D40" s="25">
+      <c r="D40" s="23">
         <v>59.99</v>
       </c>
-      <c r="E40" s="41"/>
-      <c r="F40" s="49"/>
-    </row>
-    <row r="41" spans="1:7" ht="20" customHeight="1">
-      <c r="A41" s="26" t="s">
+      <c r="E40" s="39"/>
+      <c r="F40" s="47"/>
+    </row>
+    <row r="41" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B41" s="27" t="s">
+      <c r="B41" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="C41" s="28">
+      <c r="C41" s="26">
         <v>32.5</v>
       </c>
-      <c r="D41" s="25">
+      <c r="D41" s="23">
         <v>64.989999999999995</v>
       </c>
-      <c r="E41" s="39"/>
-      <c r="F41" s="49"/>
-    </row>
-    <row r="42" spans="1:7" ht="20" customHeight="1">
-      <c r="A42" s="26" t="s">
+      <c r="E41" s="37"/>
+      <c r="F41" s="47"/>
+    </row>
+    <row r="42" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="B42" s="27" t="s">
+      <c r="B42" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="28">
+      <c r="C42" s="26">
         <v>44</v>
       </c>
-      <c r="D42" s="25">
+      <c r="D42" s="23">
         <v>89.99</v>
       </c>
-      <c r="E42" s="41"/>
-      <c r="F42" s="49"/>
-    </row>
-    <row r="43" spans="1:7" ht="20" customHeight="1">
-      <c r="A43" s="26" t="s">
+      <c r="E42" s="39"/>
+      <c r="F42" s="47"/>
+    </row>
+    <row r="43" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B43" s="27" t="s">
+      <c r="B43" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="28">
+      <c r="C43" s="26">
         <v>25</v>
       </c>
-      <c r="D43" s="25">
+      <c r="D43" s="23">
         <v>49.99</v>
       </c>
-      <c r="E43" s="39"/>
-      <c r="F43" s="49"/>
-    </row>
-    <row r="44" spans="1:7" ht="20" customHeight="1">
-      <c r="A44" s="26" t="s">
+      <c r="E43" s="37"/>
+      <c r="F43" s="47"/>
+    </row>
+    <row r="44" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="B44" s="27" t="s">
+      <c r="B44" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="C44" s="28">
+      <c r="C44" s="26">
         <v>32.5</v>
       </c>
-      <c r="D44" s="25">
+      <c r="D44" s="23">
         <v>64.989999999999995</v>
       </c>
-      <c r="E44" s="39"/>
-      <c r="F44" s="49"/>
-    </row>
-    <row r="45" spans="1:7" ht="20" customHeight="1">
-      <c r="A45" s="26" t="s">
+      <c r="E44" s="37"/>
+      <c r="F44" s="47"/>
+    </row>
+    <row r="45" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="B45" s="27" t="s">
+      <c r="B45" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="C45" s="28">
+      <c r="C45" s="26">
         <v>39.5</v>
       </c>
-      <c r="D45" s="25">
+      <c r="D45" s="23">
         <v>79.989999999999995</v>
       </c>
-      <c r="E45" s="21"/>
-      <c r="F45" s="50"/>
-      <c r="G45" s="16"/>
-    </row>
-    <row r="46" spans="1:7" ht="20" customHeight="1">
-      <c r="A46" s="26" t="s">
+      <c r="E45" s="19"/>
+      <c r="F45" s="48"/>
+      <c r="G45" s="15"/>
+    </row>
+    <row r="46" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="B46" s="29" t="s">
+      <c r="B46" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="C46" s="28">
+      <c r="C46" s="26">
         <v>48</v>
       </c>
-      <c r="D46" s="25">
+      <c r="D46" s="23">
         <v>94.99</v>
       </c>
-      <c r="E46" s="39"/>
-      <c r="F46" s="49"/>
-    </row>
-    <row r="47" spans="1:7" ht="20" customHeight="1">
-      <c r="A47" s="26" t="s">
+      <c r="E46" s="37"/>
+      <c r="F46" s="47"/>
+    </row>
+    <row r="47" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="29" t="s">
+      <c r="B47" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="C47" s="28">
+      <c r="C47" s="26">
         <v>38.5</v>
       </c>
-      <c r="D47" s="25">
+      <c r="D47" s="23">
         <v>79.989999999999995</v>
       </c>
-      <c r="E47" s="39"/>
-      <c r="F47" s="49"/>
-    </row>
-    <row r="48" spans="1:7" ht="20" customHeight="1">
-      <c r="A48" s="31" t="s">
+      <c r="E47" s="37"/>
+      <c r="F47" s="47"/>
+    </row>
+    <row r="48" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B48" s="32" t="s">
+      <c r="B48" s="30" t="s">
         <v>187</v>
       </c>
-      <c r="C48" s="28">
+      <c r="C48" s="26">
         <v>30</v>
       </c>
-      <c r="D48" s="25">
+      <c r="D48" s="23">
         <v>59.99</v>
       </c>
-      <c r="E48" s="39"/>
-      <c r="F48" s="49"/>
-    </row>
-    <row r="49" spans="1:7" ht="20" customHeight="1">
-      <c r="A49" s="31" t="s">
+      <c r="E48" s="37"/>
+      <c r="F48" s="47"/>
+    </row>
+    <row r="49" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B49" s="32" t="s">
+      <c r="B49" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="C49" s="28">
+      <c r="C49" s="26">
         <v>32</v>
       </c>
-      <c r="D49" s="25">
+      <c r="D49" s="23">
         <f>C49*2</f>
         <v>64</v>
       </c>
-      <c r="E49" s="39"/>
-      <c r="F49" s="49"/>
-    </row>
-    <row r="50" spans="1:7" ht="20" customHeight="1">
-      <c r="A50" s="31" t="s">
+      <c r="E49" s="37"/>
+      <c r="F49" s="47"/>
+    </row>
+    <row r="50" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="B50" s="32" t="s">
+      <c r="B50" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="C50" s="28">
+      <c r="C50" s="26">
         <v>32</v>
       </c>
-      <c r="D50" s="46">
+      <c r="D50" s="44">
         <v>59.99</v>
       </c>
-      <c r="E50" s="39"/>
-      <c r="F50" s="49"/>
-    </row>
-    <row r="51" spans="1:7" ht="20" customHeight="1">
-      <c r="A51" s="31" t="s">
+      <c r="E50" s="37"/>
+      <c r="F50" s="47"/>
+    </row>
+    <row r="51" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="29" t="s">
         <v>188</v>
       </c>
-      <c r="B51" s="32" t="s">
+      <c r="B51" s="30" t="s">
         <v>152</v>
       </c>
-      <c r="C51" s="28">
+      <c r="C51" s="26">
         <v>28</v>
       </c>
-      <c r="D51" s="46">
+      <c r="D51" s="44">
         <v>59.99</v>
       </c>
-      <c r="E51" s="39"/>
-      <c r="F51" s="49"/>
-    </row>
-    <row r="52" spans="1:7" ht="20" customHeight="1">
-      <c r="A52" s="31" t="s">
+      <c r="E51" s="37"/>
+      <c r="F51" s="47"/>
+    </row>
+    <row r="52" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="B52" s="32" t="s">
+      <c r="B52" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="C52" s="28">
+      <c r="C52" s="26">
         <v>26.5</v>
       </c>
-      <c r="D52" s="25">
+      <c r="D52" s="23">
         <v>54.99</v>
       </c>
-      <c r="E52" s="17"/>
-      <c r="F52" s="50"/>
-      <c r="G52" s="16"/>
-    </row>
-    <row r="53" spans="1:7" ht="20" customHeight="1">
-      <c r="A53" s="31" t="s">
+      <c r="E52" s="16"/>
+      <c r="F52" s="48"/>
+      <c r="G52" s="15"/>
+    </row>
+    <row r="53" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B53" s="33" t="s">
+      <c r="B53" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="C53" s="28">
+      <c r="C53" s="26">
         <v>25</v>
       </c>
-      <c r="D53" s="47">
+      <c r="D53" s="45">
         <v>49.99</v>
       </c>
-      <c r="E53" s="39"/>
-      <c r="F53" s="49"/>
-    </row>
-    <row r="54" spans="1:7" ht="20" customHeight="1">
-      <c r="A54" s="34" t="s">
+      <c r="E53" s="37"/>
+      <c r="F53" s="47"/>
+    </row>
+    <row r="54" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="B54" s="32" t="s">
+      <c r="B54" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C54" s="28">
+      <c r="C54" s="26">
         <v>32</v>
       </c>
-      <c r="D54" s="47">
+      <c r="D54" s="45">
         <f>C54*2</f>
         <v>64</v>
       </c>
-      <c r="E54" s="39"/>
-      <c r="F54" s="49"/>
-    </row>
-    <row r="55" spans="1:7" ht="20" customHeight="1">
-      <c r="A55" s="31" t="s">
+      <c r="E54" s="37"/>
+      <c r="F54" s="47"/>
+    </row>
+    <row r="55" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="B55" s="33" t="s">
+      <c r="B55" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="C55" s="28">
+      <c r="C55" s="26">
         <v>42</v>
       </c>
-      <c r="D55" s="47">
+      <c r="D55" s="45">
         <f>C55*2</f>
         <v>84</v>
       </c>
-      <c r="E55" s="39"/>
-      <c r="F55" s="49"/>
-    </row>
-    <row r="56" spans="1:7" ht="20" customHeight="1">
-      <c r="A56" s="34" t="s">
+      <c r="E55" s="37"/>
+      <c r="F55" s="47"/>
+    </row>
+    <row r="56" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="B56" s="32" t="s">
+      <c r="B56" s="30" t="s">
         <v>189</v>
       </c>
-      <c r="C56" s="28">
+      <c r="C56" s="26">
         <v>35</v>
       </c>
-      <c r="D56" s="47">
+      <c r="D56" s="45">
         <v>69.989999999999995</v>
       </c>
-      <c r="E56" s="39"/>
-      <c r="F56" s="49"/>
-    </row>
-    <row r="57" spans="1:7" s="35" customFormat="1" ht="20" customHeight="1">
-      <c r="A57" s="24" t="s">
+      <c r="E56" s="37"/>
+      <c r="F56" s="47"/>
+    </row>
+    <row r="57" spans="1:7" s="33" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B57" s="30" t="s">
+      <c r="B57" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="C57" s="25">
+      <c r="C57" s="23">
         <v>22</v>
       </c>
-      <c r="D57" s="44">
+      <c r="D57" s="42">
         <v>49.99</v>
       </c>
-      <c r="E57" s="39"/>
-      <c r="F57" s="49"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="47"/>
       <c r="G57" s="3"/>
     </row>
-    <row r="58" spans="1:7" ht="20" customHeight="1">
-      <c r="A58" s="31" t="s">
+    <row r="58" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="B58" s="33" t="s">
+      <c r="B58" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="C58" s="28">
+      <c r="C58" s="26">
         <v>31</v>
       </c>
-      <c r="D58" s="47">
+      <c r="D58" s="45">
         <v>59.99</v>
       </c>
-      <c r="E58" s="39"/>
-      <c r="F58" s="49"/>
-    </row>
-    <row r="59" spans="1:7" ht="20" customHeight="1">
-      <c r="A59" s="24" t="s">
+      <c r="E58" s="37"/>
+      <c r="F58" s="47"/>
+    </row>
+    <row r="59" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="B59" s="24" t="s">
+      <c r="B59" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="C59" s="25">
+      <c r="C59" s="23">
         <v>32</v>
       </c>
-      <c r="D59" s="44">
+      <c r="D59" s="42">
         <v>59.99</v>
       </c>
-      <c r="E59" s="39"/>
-      <c r="F59" s="49"/>
-    </row>
-    <row r="60" spans="1:7" ht="20" customHeight="1">
-      <c r="A60" s="26" t="s">
+      <c r="E59" s="37"/>
+      <c r="F59" s="47"/>
+    </row>
+    <row r="60" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="B60" s="27" t="s">
+      <c r="B60" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="C60" s="25">
+      <c r="C60" s="23">
         <v>24</v>
       </c>
-      <c r="D60" s="25">
+      <c r="D60" s="23">
         <v>49.99</v>
       </c>
-      <c r="E60" s="42"/>
-      <c r="F60" s="49"/>
-    </row>
-    <row r="61" spans="1:7" ht="20" customHeight="1">
-      <c r="A61" s="26" t="s">
+      <c r="E60" s="40"/>
+      <c r="F60" s="47"/>
+    </row>
+    <row r="61" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="B61" s="29" t="s">
+      <c r="B61" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="C61" s="28">
+      <c r="C61" s="26">
         <v>24</v>
       </c>
-      <c r="D61" s="47">
+      <c r="D61" s="45">
         <v>49.99</v>
       </c>
-      <c r="E61" s="39"/>
-      <c r="F61" s="49"/>
-    </row>
-    <row r="62" spans="1:7" ht="20" customHeight="1">
-      <c r="A62" s="24" t="s">
+      <c r="E61" s="37"/>
+      <c r="F61" s="47"/>
+    </row>
+    <row r="62" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="B62" s="30" t="s">
+      <c r="B62" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="C62" s="25">
+      <c r="C62" s="23">
         <v>25</v>
       </c>
-      <c r="D62" s="44">
+      <c r="D62" s="42">
         <v>49.99</v>
       </c>
-      <c r="E62" s="39"/>
-      <c r="F62" s="49"/>
-    </row>
-    <row r="63" spans="1:7" ht="20" customHeight="1">
-      <c r="A63" s="31" t="s">
+      <c r="E62" s="37"/>
+      <c r="F62" s="47"/>
+    </row>
+    <row r="63" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="B63" s="33" t="s">
+      <c r="B63" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="C63" s="28">
+      <c r="C63" s="26">
         <v>25</v>
       </c>
-      <c r="D63" s="25">
+      <c r="D63" s="23">
         <v>49.99</v>
       </c>
-      <c r="E63" s="48"/>
-      <c r="F63" s="51"/>
-      <c r="G63" s="35"/>
-    </row>
-    <row r="64" spans="1:7" ht="20" customHeight="1">
-      <c r="A64" s="31" t="s">
+      <c r="E63" s="46"/>
+      <c r="F63" s="49"/>
+      <c r="G63" s="33"/>
+    </row>
+    <row r="64" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="B64" s="33" t="s">
+      <c r="B64" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="C64" s="28">
+      <c r="C64" s="26">
         <v>32</v>
       </c>
-      <c r="D64" s="25">
+      <c r="D64" s="23">
         <v>59.99</v>
       </c>
-      <c r="E64" s="39"/>
-      <c r="F64" s="49"/>
-    </row>
-    <row r="65" spans="1:6" ht="20" customHeight="1">
-      <c r="A65" s="31" t="s">
+      <c r="E64" s="37"/>
+      <c r="F64" s="47"/>
+    </row>
+    <row r="65" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="B65" s="33" t="s">
+      <c r="B65" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="C65" s="28">
+      <c r="C65" s="26">
         <v>28.5</v>
       </c>
-      <c r="D65" s="25">
+      <c r="D65" s="23">
         <v>59.99</v>
       </c>
-      <c r="E65" s="39"/>
-      <c r="F65" s="49"/>
-    </row>
-    <row r="66" spans="1:6" ht="20" customHeight="1">
-      <c r="A66" s="31" t="s">
+      <c r="E65" s="37"/>
+      <c r="F65" s="47"/>
+    </row>
+    <row r="66" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="B66" s="33" t="s">
+      <c r="B66" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="C66" s="28">
+      <c r="C66" s="26">
         <v>32</v>
       </c>
-      <c r="D66" s="25">
+      <c r="D66" s="23">
         <v>59.99</v>
       </c>
-      <c r="E66" s="41"/>
-      <c r="F66" s="49"/>
-    </row>
-    <row r="67" spans="1:6" ht="20" customHeight="1" thickBot="1">
-      <c r="A67" s="31" t="s">
+      <c r="E66" s="39"/>
+      <c r="F66" s="47"/>
+    </row>
+    <row r="67" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="B67" s="33" t="s">
+      <c r="B67" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="C67" s="28">
+      <c r="C67" s="26">
         <v>24</v>
       </c>
-      <c r="D67" s="25">
+      <c r="D67" s="23">
         <v>49.99</v>
       </c>
-      <c r="E67" s="39"/>
-      <c r="F67" s="49"/>
-    </row>
-    <row r="68" spans="1:6" ht="20" customHeight="1" thickBot="1">
-      <c r="E68" s="54" t="s">
+      <c r="E67" s="37"/>
+      <c r="F67" s="47"/>
+    </row>
+    <row r="68" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E68" s="52" t="s">
         <v>180</v>
       </c>
-      <c r="F68" s="55"/>
-    </row>
-    <row r="69" spans="1:6" ht="20" customHeight="1"/>
-    <row r="70" spans="1:6" ht="20" customHeight="1"/>
-    <row r="71" spans="1:6" ht="20" customHeight="1"/>
-    <row r="72" spans="1:6" ht="20" customHeight="1"/>
-    <row r="73" spans="1:6" ht="20" customHeight="1"/>
-    <row r="74" spans="1:6" ht="20" customHeight="1"/>
-    <row r="75" spans="1:6" ht="20" customHeight="1"/>
-    <row r="76" spans="1:6" ht="20" customHeight="1"/>
-    <row r="77" spans="1:6" ht="20" customHeight="1"/>
-    <row r="78" spans="1:6" ht="20" customHeight="1"/>
-    <row r="79" spans="1:6" ht="20" customHeight="1"/>
+      <c r="F68" s="53"/>
+    </row>
+    <row r="69" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sortState ref="A2:L275">
     <sortCondition ref="A2:A275"/>
@@ -2627,25 +2669,25 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="82.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" style="19" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="19" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="4" hidden="1" customWidth="1"/>
-    <col min="7" max="16384" width="17.33203125" style="3"/>
+    <col min="1" max="1" width="82.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="18" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="18" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="7" max="16384" width="17.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" customHeight="1" thickBot="1">
+    <row r="1" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2658,62 +2700,62 @@
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="50" t="s">
         <v>179</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="51" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="23">
         <v>10</v>
       </c>
-      <c r="D2" s="44">
+      <c r="D2" s="42">
         <v>19.989999999999998</v>
       </c>
-      <c r="E2" s="39"/>
-      <c r="F2" s="49"/>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1" thickBot="1">
-      <c r="A3" s="24" t="s">
+      <c r="E2" s="37"/>
+      <c r="F2" s="47"/>
+    </row>
+    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="23">
         <v>10</v>
       </c>
-      <c r="D3" s="44">
+      <c r="D3" s="42">
         <v>19.989999999999998</v>
       </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="49"/>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1" thickBot="1">
-      <c r="E4" s="54" t="s">
+      <c r="E3" s="37"/>
+      <c r="F3" s="47"/>
+    </row>
+    <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E4" s="52" t="s">
         <v>180</v>
       </c>
-      <c r="F4" s="55"/>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1"/>
-    <row r="6" spans="1:6" ht="20" customHeight="1"/>
-    <row r="7" spans="1:6" ht="20" customHeight="1"/>
-    <row r="8" spans="1:6" ht="20" customHeight="1"/>
-    <row r="9" spans="1:6" ht="20" customHeight="1"/>
-    <row r="10" spans="1:6" ht="20" customHeight="1"/>
-    <row r="11" spans="1:6" ht="20" customHeight="1"/>
-    <row r="12" spans="1:6" ht="20" customHeight="1"/>
-    <row r="13" spans="1:6" ht="20" customHeight="1"/>
-    <row r="14" spans="1:6" ht="20" customHeight="1"/>
-    <row r="15" spans="1:6" ht="20" customHeight="1"/>
+      <c r="F4" s="53"/>
+    </row>
+    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.2" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="35" fitToHeight="13" orientation="portrait"/>
@@ -2737,18 +2779,18 @@
       <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="82.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" style="19" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="19" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="4" hidden="1" customWidth="1"/>
-    <col min="7" max="16384" width="17.33203125" style="3"/>
+    <col min="1" max="1" width="82.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="18" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="18" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="7" max="16384" width="17.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" customHeight="1" thickBot="1">
+    <row r="1" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2761,179 +2803,179 @@
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="50" t="s">
         <v>179</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="51" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="20" customHeight="1">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="28">
+      <c r="C2" s="26">
         <v>4.5</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="23">
         <v>9.99</v>
       </c>
-      <c r="E2" s="39"/>
-      <c r="F2" s="49"/>
-    </row>
-    <row r="3" spans="1:7" ht="20" customHeight="1">
-      <c r="A3" s="34" t="s">
+      <c r="E2" s="37"/>
+      <c r="F2" s="47"/>
+    </row>
+    <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="26">
         <v>5</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="23">
         <f>C3*2</f>
         <v>10</v>
       </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="49"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="47"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="20" customHeight="1">
-      <c r="A4" s="31" t="s">
+    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="26">
         <v>4.5</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="23">
         <v>9.99</v>
       </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="49"/>
-    </row>
-    <row r="5" spans="1:7" ht="20" customHeight="1">
-      <c r="A5" s="31" t="s">
+      <c r="E4" s="37"/>
+      <c r="F4" s="47"/>
+    </row>
+    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="26">
         <v>4</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="23">
         <v>9.99</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="16"/>
-    </row>
-    <row r="6" spans="1:7" ht="20" customHeight="1">
-      <c r="A6" s="31" t="s">
+      <c r="E5" s="20"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="15"/>
+    </row>
+    <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="26">
         <v>4</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="23">
         <v>9.99</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="16"/>
-    </row>
-    <row r="7" spans="1:7" ht="20" customHeight="1">
-      <c r="A7" s="31" t="s">
+      <c r="E6" s="16"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="15"/>
+    </row>
+    <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="26">
         <v>4.5</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="23">
         <v>9.99</v>
       </c>
-      <c r="E7" s="39"/>
-      <c r="F7" s="49"/>
-    </row>
-    <row r="8" spans="1:7" ht="20" customHeight="1">
-      <c r="A8" s="31" t="s">
+      <c r="E7" s="37"/>
+      <c r="F7" s="47"/>
+    </row>
+    <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="26">
         <v>4</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="23">
         <v>9.99</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="16"/>
-    </row>
-    <row r="9" spans="1:7" ht="20" customHeight="1">
-      <c r="A9" s="31" t="s">
+      <c r="E8" s="16"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="26">
         <v>4</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="23">
         <v>9.99</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="49"/>
-    </row>
-    <row r="10" spans="1:7" ht="20" customHeight="1" thickBot="1">
-      <c r="A10" s="31" t="s">
+      <c r="E9" s="37"/>
+      <c r="F9" s="47"/>
+    </row>
+    <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="26">
         <v>5</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="23">
         <v>9.99</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="49"/>
-    </row>
-    <row r="11" spans="1:7" ht="20" customHeight="1" thickBot="1">
-      <c r="E11" s="54" t="s">
+      <c r="E10" s="37"/>
+      <c r="F10" s="47"/>
+    </row>
+    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E11" s="52" t="s">
         <v>180</v>
       </c>
-      <c r="F11" s="55"/>
-    </row>
-    <row r="12" spans="1:7" ht="20" customHeight="1"/>
-    <row r="13" spans="1:7" ht="20" customHeight="1"/>
-    <row r="14" spans="1:7" ht="20" customHeight="1"/>
-    <row r="15" spans="1:7" ht="20" customHeight="1"/>
-    <row r="16" spans="1:7" ht="20" customHeight="1"/>
-    <row r="17" ht="20" customHeight="1"/>
-    <row r="18" ht="20" customHeight="1"/>
-    <row r="19" ht="20" customHeight="1"/>
-    <row r="20" ht="20" customHeight="1"/>
-    <row r="21" ht="20" customHeight="1"/>
-    <row r="22" ht="20" customHeight="1"/>
+      <c r="F11" s="53"/>
+    </row>
+    <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.2" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="35" fitToHeight="13" orientation="portrait"/>
@@ -2950,25 +2992,25 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="82.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" style="19" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="19" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="4" hidden="1" customWidth="1"/>
-    <col min="7" max="16384" width="17.33203125" style="3"/>
+    <col min="1" max="1" width="82.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="18" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="18" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="7" max="16384" width="17.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" customHeight="1" thickBot="1">
+    <row r="1" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2981,128 +3023,128 @@
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="50" t="s">
         <v>179</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="51" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>20</v>
       </c>
-      <c r="D2" s="40">
+      <c r="D2" s="38">
         <v>39.99</v>
       </c>
-      <c r="E2" s="39"/>
-      <c r="F2" s="49"/>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
-      <c r="A3" s="26" t="s">
+      <c r="E2" s="37"/>
+      <c r="F2" s="47"/>
+    </row>
+    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="26">
         <v>22</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="23">
         <f>C3*2</f>
         <v>44</v>
       </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="49"/>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="E3" s="37"/>
+      <c r="F3" s="47"/>
+    </row>
+    <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="26">
         <v>26</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="23">
         <v>54.99</v>
       </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="49"/>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1">
-      <c r="A5" s="31" t="s">
+      <c r="E4" s="37"/>
+      <c r="F4" s="47"/>
+    </row>
+    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="26">
         <v>22.5</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="23">
         <f>C5*2</f>
         <v>45</v>
       </c>
-      <c r="E5" s="39"/>
-      <c r="F5" s="49"/>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1">
-      <c r="A6" s="30" t="s">
+      <c r="E5" s="37"/>
+      <c r="F5" s="47"/>
+    </row>
+    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="23">
         <v>35</v>
       </c>
-      <c r="D6" s="44">
+      <c r="D6" s="42">
         <v>69.989999999999995</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="49"/>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1" thickBot="1">
-      <c r="A7" s="31" t="s">
+      <c r="E6" s="37"/>
+      <c r="F6" s="47"/>
+    </row>
+    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="26">
         <v>25</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="23">
         <v>49.99</v>
       </c>
-      <c r="E7" s="39"/>
-      <c r="F7" s="49"/>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1" thickBot="1">
-      <c r="E8" s="54" t="s">
+      <c r="E7" s="37"/>
+      <c r="F7" s="47"/>
+    </row>
+    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E8" s="52" t="s">
         <v>180</v>
       </c>
-      <c r="F8" s="55"/>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1"/>
-    <row r="10" spans="1:6" ht="20" customHeight="1"/>
-    <row r="11" spans="1:6" ht="20" customHeight="1"/>
-    <row r="12" spans="1:6" ht="20" customHeight="1"/>
-    <row r="13" spans="1:6" ht="20" customHeight="1"/>
-    <row r="14" spans="1:6" ht="20" customHeight="1"/>
-    <row r="15" spans="1:6" ht="20" customHeight="1"/>
-    <row r="16" spans="1:6" ht="20" customHeight="1"/>
-    <row r="17" ht="20" customHeight="1"/>
-    <row r="18" ht="20" customHeight="1"/>
-    <row r="19" ht="20" customHeight="1"/>
+      <c r="F8" s="53"/>
+    </row>
+    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.2" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="35" fitToHeight="13" orientation="portrait"/>
@@ -3126,18 +3168,18 @@
       <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="82.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" style="19" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="19" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="4" hidden="1" customWidth="1"/>
-    <col min="7" max="16384" width="17.33203125" style="3"/>
+    <col min="1" max="1" width="82.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="18" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="18" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="7" max="16384" width="17.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" customHeight="1" thickBot="1">
+    <row r="1" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3150,58 +3192,58 @@
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="50" t="s">
         <v>179</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="51" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="28">
+      <c r="C2" s="26">
         <v>8.25</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="23">
         <f>C2*2</f>
         <v>16.5</v>
       </c>
-      <c r="E2" s="39"/>
-      <c r="F2" s="49"/>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
-      <c r="A3" s="31" t="s">
+      <c r="E2" s="37"/>
+      <c r="F2" s="47"/>
+    </row>
+    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="26">
         <v>7.5</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="23">
         <f>C3*2</f>
         <v>15</v>
       </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="49"/>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1"/>
-    <row r="5" spans="1:6" ht="20" customHeight="1"/>
-    <row r="6" spans="1:6" ht="20" customHeight="1"/>
-    <row r="7" spans="1:6" ht="20" customHeight="1"/>
-    <row r="8" spans="1:6" ht="20" customHeight="1"/>
-    <row r="9" spans="1:6" ht="20" customHeight="1"/>
-    <row r="10" spans="1:6" ht="20" customHeight="1"/>
-    <row r="11" spans="1:6" ht="20" customHeight="1"/>
-    <row r="12" spans="1:6" ht="20" customHeight="1"/>
-    <row r="13" spans="1:6" ht="20" customHeight="1"/>
-    <row r="14" spans="1:6" ht="20" customHeight="1"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="47"/>
+    </row>
+    <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.2" right="0" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="35" fitToHeight="13" orientation="portrait"/>
@@ -3225,18 +3267,18 @@
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="82.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" style="19" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="19" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="4" hidden="1" customWidth="1"/>
-    <col min="7" max="16384" width="17.33203125" style="3"/>
+    <col min="1" max="1" width="82.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="18" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="18" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="7" max="16384" width="17.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" customHeight="1" thickBot="1">
+    <row r="1" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3249,231 +3291,231 @@
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="50" t="s">
         <v>179</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="51" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="20" customHeight="1">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>140</v>
       </c>
-      <c r="D2" s="40">
+      <c r="D2" s="38">
         <v>189.99</v>
       </c>
-      <c r="E2" s="39"/>
-      <c r="F2" s="49"/>
-    </row>
-    <row r="3" spans="1:7" ht="20" customHeight="1">
-      <c r="A3" s="11" t="s">
+      <c r="E2" s="37"/>
+      <c r="F2" s="47"/>
+    </row>
+    <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>140</v>
       </c>
-      <c r="D3" s="40">
+      <c r="D3" s="38">
         <v>189.99</v>
       </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="49"/>
-    </row>
-    <row r="4" spans="1:7" ht="20" customHeight="1">
-      <c r="A4" s="13" t="s">
+      <c r="E3" s="37"/>
+      <c r="F3" s="47"/>
+    </row>
+    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="13">
         <v>10</v>
       </c>
-      <c r="D4" s="38">
+      <c r="D4" s="36">
         <v>19.989999999999998</v>
       </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="49"/>
-    </row>
-    <row r="5" spans="1:7" ht="20" customHeight="1">
-      <c r="A5" s="17" t="s">
+      <c r="E4" s="37"/>
+      <c r="F4" s="47"/>
+    </row>
+    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="17">
         <v>20.5</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <v>39.99</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="49"/>
-    </row>
-    <row r="6" spans="1:7" ht="20" customHeight="1">
+      <c r="E5" s="40"/>
+      <c r="F5" s="47"/>
+    </row>
+    <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>25</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="36">
         <v>49.99</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="49"/>
-    </row>
-    <row r="7" spans="1:7" ht="20" customHeight="1">
-      <c r="A7" s="31" t="s">
+      <c r="E6" s="37"/>
+      <c r="F6" s="47"/>
+    </row>
+    <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="26">
         <v>5</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="23">
         <v>9.99</v>
       </c>
-      <c r="E7" s="39"/>
-      <c r="F7" s="49"/>
-    </row>
-    <row r="8" spans="1:7" ht="20" customHeight="1">
-      <c r="A8" s="31" t="s">
+      <c r="E7" s="37"/>
+      <c r="F7" s="47"/>
+    </row>
+    <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="26">
         <v>5</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="23">
         <v>9.99</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="16"/>
-    </row>
-    <row r="9" spans="1:7" ht="20" customHeight="1">
-      <c r="A9" s="31" t="s">
+      <c r="E8" s="16"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="26">
         <v>38</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="23">
         <v>74.989999999999995</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="49"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="47"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" ht="20" customHeight="1">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="13">
         <v>20</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="36">
         <v>39.99</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="49"/>
-    </row>
-    <row r="11" spans="1:7" ht="20" customHeight="1"/>
-    <row r="12" spans="1:7" ht="20" customHeight="1"/>
-    <row r="13" spans="1:7" ht="20" customHeight="1"/>
-    <row r="14" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1">
+      <c r="E10" s="37"/>
+      <c r="F10" s="47"/>
+    </row>
+    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:7" s="35" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
       <c r="F14" s="4"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1">
+    <row r="15" spans="1:7" s="35" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
       <c r="F15" s="4"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1">
+    <row r="16" spans="1:7" s="35" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
       <c r="F16" s="4"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1">
+    <row r="17" spans="1:7" s="35" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="4"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1">
+    <row r="18" spans="1:7" s="35" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
       <c r="F18" s="4"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1">
+    <row r="19" spans="1:7" s="35" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
       <c r="F19" s="4"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1">
+    <row r="20" spans="1:7" s="35" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
       <c r="F20" s="4"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" s="37" customFormat="1" ht="20" customHeight="1">
+    <row r="21" spans="1:7" s="35" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
       <c r="F21" s="4"/>
       <c r="G21" s="3"/>
     </row>

</xml_diff>